<commit_message>
Added last couple team meetings plus updated Gantt chart
</commit_message>
<xml_diff>
--- a/docs/Equifoods Gantt.xlsx
+++ b/docs/Equifoods Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD23778-FBA8-4104-9A2D-B1D9A735B515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF5F90-31A4-4B63-9A84-35E41CA2D9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>Task 3</t>
   </si>
@@ -213,6 +213,45 @@
   </si>
   <si>
     <t>Equifood</t>
+  </si>
+  <si>
+    <t>Add map view</t>
+  </si>
+  <si>
+    <t>Shopping cart button</t>
+  </si>
+  <si>
+    <t>Loading screen</t>
+  </si>
+  <si>
+    <t>Merchant page</t>
+  </si>
+  <si>
+    <t>Orders page</t>
+  </si>
+  <si>
+    <t>Restaurant filters</t>
+  </si>
+  <si>
+    <t>Jordon R</t>
+  </si>
+  <si>
+    <t>Make merchant page look nice</t>
+  </si>
+  <si>
+    <t>Improve map page</t>
+  </si>
+  <si>
+    <t>Account page</t>
+  </si>
+  <si>
+    <t>Fi</t>
+  </si>
+  <si>
+    <t>Fix action sheet on map page</t>
+  </si>
+  <si>
+    <t>Change app to single item based</t>
   </si>
 </sst>
 </file>
@@ -808,23 +847,23 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1336,28 +1375,28 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL41"/>
+  <dimension ref="A1:BL52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="101" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="48" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5703125" customWidth="1"/>
-    <col min="69" max="70" width="10.28515625"/>
+    <col min="1" max="1" width="2.69140625" style="48" customWidth="1"/>
+    <col min="2" max="2" width="57.53515625" customWidth="1"/>
+    <col min="3" max="3" width="30.69140625" customWidth="1"/>
+    <col min="4" max="4" width="10.69140625" customWidth="1"/>
+    <col min="5" max="5" width="10.3828125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.3828125" customWidth="1"/>
+    <col min="7" max="7" width="2.69140625" customWidth="1"/>
+    <col min="8" max="8" width="6.15234375" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.53515625" customWidth="1"/>
+    <col min="69" max="70" width="10.3046875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="49" t="s">
         <v>18</v>
       </c>
@@ -1371,120 +1410,120 @@
       <c r="H1" s="2"/>
       <c r="I1" s="75"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="48" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="53"/>
       <c r="I2" s="76"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="48" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="54"/>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="82">
+      <c r="D3" s="82"/>
+      <c r="E3" s="80">
         <v>44844</v>
       </c>
-      <c r="F3" s="82"/>
+      <c r="F3" s="80"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="78"/>
+      <c r="D4" s="82"/>
       <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="I4" s="79">
+      <c r="I4" s="77">
         <f>I5</f>
         <v>44851</v>
       </c>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="79">
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="77">
         <f>P5</f>
         <v>44858</v>
       </c>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="79">
+      <c r="Q4" s="78"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="77">
         <f>W5</f>
         <v>44865</v>
       </c>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="80"/>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="79">
+      <c r="X4" s="78"/>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="77">
         <f>AD5</f>
         <v>44872</v>
       </c>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="80"/>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="80"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="79">
+      <c r="AE4" s="78"/>
+      <c r="AF4" s="78"/>
+      <c r="AG4" s="78"/>
+      <c r="AH4" s="78"/>
+      <c r="AI4" s="78"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="77">
         <f>AK5</f>
         <v>44879</v>
       </c>
-      <c r="AL4" s="80"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="80"/>
-      <c r="AO4" s="80"/>
-      <c r="AP4" s="80"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="79">
+      <c r="AL4" s="78"/>
+      <c r="AM4" s="78"/>
+      <c r="AN4" s="78"/>
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="77">
         <f>AR5</f>
         <v>44886</v>
       </c>
-      <c r="AS4" s="80"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="80"/>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="80"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="79">
+      <c r="AS4" s="78"/>
+      <c r="AT4" s="78"/>
+      <c r="AU4" s="78"/>
+      <c r="AV4" s="78"/>
+      <c r="AW4" s="78"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="77">
         <f>AY5</f>
         <v>44893</v>
       </c>
-      <c r="AZ4" s="80"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="80"/>
-      <c r="BC4" s="80"/>
-      <c r="BD4" s="80"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="79">
+      <c r="AZ4" s="78"/>
+      <c r="BA4" s="78"/>
+      <c r="BB4" s="78"/>
+      <c r="BC4" s="78"/>
+      <c r="BD4" s="78"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="77">
         <f>BF5</f>
         <v>44900</v>
       </c>
-      <c r="BG4" s="80"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="80"/>
-      <c r="BJ4" s="80"/>
-      <c r="BK4" s="80"/>
-      <c r="BL4" s="81"/>
+      <c r="BG4" s="78"/>
+      <c r="BH4" s="78"/>
+      <c r="BI4" s="78"/>
+      <c r="BJ4" s="78"/>
+      <c r="BK4" s="78"/>
+      <c r="BL4" s="79"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="49" t="s">
         <v>20</v>
       </c>
@@ -1719,7 +1758,7 @@
         <v>44906</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="49" t="s">
         <v>21</v>
       </c>
@@ -1967,7 +2006,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="48" t="s">
         <v>26</v>
       </c>
@@ -2034,7 +2073,7 @@
       <c r="BK7" s="44"/>
       <c r="BL7" s="44"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="49" t="s">
         <v>22</v>
       </c>
@@ -2047,7 +2086,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="str">
-        <f t="shared" ref="H8:H38" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H49" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="44"/>
@@ -2107,7 +2146,7 @@
       <c r="BK8" s="44"/>
       <c r="BL8" s="44"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="49" t="s">
         <v>27</v>
       </c>
@@ -2125,7 +2164,7 @@
         <v>44857</v>
       </c>
       <c r="F9" s="55">
-        <f t="shared" ref="F9:F18" si="7">E9+3</f>
+        <f t="shared" ref="F9:F20" si="7">E9+3</f>
         <v>44860</v>
       </c>
       <c r="G9" s="17"/>
@@ -2190,7 +2229,7 @@
       <c r="BK9" s="44"/>
       <c r="BL9" s="44"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="49" t="s">
         <v>23</v>
       </c>
@@ -2273,7 +2312,7 @@
       <c r="BK10" s="44"/>
       <c r="BL10" s="44"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="48"/>
       <c r="B11" s="69" t="s">
         <v>35</v>
@@ -2354,7 +2393,7 @@
       <c r="BK11" s="44"/>
       <c r="BL11" s="44"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="48"/>
       <c r="B12" s="69" t="s">
         <v>36</v>
@@ -2435,7 +2474,7 @@
       <c r="BK12" s="44"/>
       <c r="BL12" s="44"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="48"/>
       <c r="B13" s="69" t="s">
         <v>37</v>
@@ -2513,7 +2552,7 @@
       <c r="BK13" s="44"/>
       <c r="BL13" s="44"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="48"/>
       <c r="B14" s="69" t="s">
         <v>38</v>
@@ -2594,7 +2633,7 @@
       <c r="BK14" s="44"/>
       <c r="BL14" s="44"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="48"/>
       <c r="B15" s="69" t="s">
         <v>39</v>
@@ -2672,7 +2711,7 @@
       <c r="BK15" s="44"/>
       <c r="BL15" s="44"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="48"/>
       <c r="B16" s="69" t="s">
         <v>40</v>
@@ -2681,7 +2720,7 @@
         <v>45</v>
       </c>
       <c r="D16" s="22">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E16" s="55">
         <f>DATE(2022, 10, 26)</f>
@@ -2750,7 +2789,7 @@
       <c r="BK16" s="44"/>
       <c r="BL16" s="44"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="48"/>
       <c r="B17" s="69" t="s">
         <v>41</v>
@@ -2759,7 +2798,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="22">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E17" s="55">
         <f>DATE(2022, 11, 2)</f>
@@ -2828,24 +2867,24 @@
       <c r="BK17" s="44"/>
       <c r="BL17" s="44"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="48"/>
       <c r="B18" s="69" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C18" s="61" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D18" s="22">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E18" s="55">
-        <f>DATE(2022, 11, 2)</f>
-        <v>44867</v>
+        <f>DATE(2022, 11, 14)</f>
+        <v>44879</v>
       </c>
       <c r="F18" s="55">
-        <f t="shared" si="7"/>
-        <v>44870</v>
+        <f>DATE(2022, 11, 17)</f>
+        <v>44882</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
@@ -2906,22 +2945,27 @@
       <c r="BK18" s="44"/>
       <c r="BL18" s="44"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="48"/>
+      <c r="B19" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="22">
+        <v>1</v>
+      </c>
+      <c r="E19" s="55">
+        <f>DATE(2022, 11, 17)</f>
+        <v>44882</v>
+      </c>
+      <c r="F19" s="55">
+        <f>DATE(2022, 11, 20)</f>
+        <v>44885</v>
+      </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H19" s="17"/>
       <c r="I19" s="44"/>
       <c r="J19" s="44"/>
       <c r="K19" s="44"/>
@@ -2979,20 +3023,27 @@
       <c r="BK19" s="44"/>
       <c r="BL19" s="44"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="48"/>
+      <c r="B20" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="22">
+        <v>1</v>
+      </c>
+      <c r="E20" s="55">
+        <f>DATE(2022, 11, 2)</f>
+        <v>44867</v>
+      </c>
+      <c r="F20" s="55">
+        <f t="shared" si="7"/>
+        <v>44870</v>
+      </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H20" s="17"/>
       <c r="I20" s="44"/>
       <c r="J20" s="44"/>
       <c r="K20" s="44"/>
@@ -3050,20 +3101,27 @@
       <c r="BK20" s="44"/>
       <c r="BL20" s="44"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="48"/>
-      <c r="B21" s="70" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
+      <c r="B21" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="22">
+        <v>1</v>
+      </c>
+      <c r="E21" s="55">
+        <f>DATE(2022, 11, 14)</f>
+        <v>44879</v>
+      </c>
+      <c r="F21" s="55">
+        <f>DATE(2022, 11, 17)</f>
+        <v>44882</v>
+      </c>
       <c r="G21" s="17"/>
-      <c r="H21" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H21" s="17"/>
       <c r="I21" s="44"/>
       <c r="J21" s="44"/>
       <c r="K21" s="44"/>
@@ -3076,8 +3134,8 @@
       <c r="R21" s="44"/>
       <c r="S21" s="44"/>
       <c r="T21" s="44"/>
-      <c r="U21" s="45"/>
-      <c r="V21" s="45"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
       <c r="W21" s="44"/>
       <c r="X21" s="44"/>
       <c r="Y21" s="44"/>
@@ -3121,20 +3179,27 @@
       <c r="BK21" s="44"/>
       <c r="BL21" s="44"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="48"/>
-      <c r="B22" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
+      <c r="B22" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="55">
+        <f>DATE(2022, 11, 14)</f>
+        <v>44879</v>
+      </c>
+      <c r="F22" s="55">
+        <f>DATE(2022, 11, 17)</f>
+        <v>44882</v>
+      </c>
       <c r="G22" s="17"/>
-      <c r="H22" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H22" s="17"/>
       <c r="I22" s="44"/>
       <c r="J22" s="44"/>
       <c r="K22" s="44"/>
@@ -3192,20 +3257,27 @@
       <c r="BK22" s="44"/>
       <c r="BL22" s="44"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="48"/>
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="22">
         <v>1</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
+      <c r="E23" s="55">
+        <f>DATE(2022, 11, 14)</f>
+        <v>44879</v>
+      </c>
+      <c r="F23" s="55">
+        <f>DATE(2022, 11, 17)</f>
+        <v>44882</v>
+      </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H23" s="17"/>
       <c r="I23" s="44"/>
       <c r="J23" s="44"/>
       <c r="K23" s="44"/>
@@ -3222,7 +3294,7 @@
       <c r="V23" s="44"/>
       <c r="W23" s="44"/>
       <c r="X23" s="44"/>
-      <c r="Y23" s="45"/>
+      <c r="Y23" s="44"/>
       <c r="Z23" s="44"/>
       <c r="AA23" s="44"/>
       <c r="AB23" s="44"/>
@@ -3263,20 +3335,27 @@
       <c r="BK23" s="44"/>
       <c r="BL23" s="44"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="48"/>
-      <c r="B24" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
+      <c r="B24" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="55">
+        <f>DATE(2022, 11, 21)</f>
+        <v>44886</v>
+      </c>
+      <c r="F24" s="55">
+        <f>DATE(2022, 11, 24)</f>
+        <v>44889</v>
+      </c>
       <c r="G24" s="17"/>
-      <c r="H24" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H24" s="17"/>
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
@@ -3334,22 +3413,27 @@
       <c r="BK24" s="44"/>
       <c r="BL24" s="44"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="64"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="48"/>
+      <c r="B25" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="22">
+        <v>1</v>
+      </c>
+      <c r="E25" s="55">
+        <f>DATE(2022, 11, 17)</f>
+        <v>44882</v>
+      </c>
+      <c r="F25" s="55">
+        <f>DATE(2022, 11, 20)</f>
+        <v>44885</v>
+      </c>
       <c r="G25" s="17"/>
-      <c r="H25" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H25" s="17"/>
       <c r="I25" s="44"/>
       <c r="J25" s="44"/>
       <c r="K25" s="44"/>
@@ -3407,20 +3491,27 @@
       <c r="BK25" s="44"/>
       <c r="BL25" s="44"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="48"/>
-      <c r="B26" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
+      <c r="B26" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="E26" s="55">
+        <f>DATE(2022, 11, 21)</f>
+        <v>44886</v>
+      </c>
+      <c r="F26" s="55">
+        <f>DATE(2022, 11, 24)</f>
+        <v>44889</v>
+      </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H26" s="17"/>
       <c r="I26" s="44"/>
       <c r="J26" s="44"/>
       <c r="K26" s="44"/>
@@ -3478,20 +3569,29 @@
       <c r="BK26" s="44"/>
       <c r="BL26" s="44"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="48"/>
-      <c r="B27" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="65"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="22">
+        <v>1</v>
+      </c>
+      <c r="E27" s="55">
+        <f>DATE(2022, 11, 24)</f>
+        <v>44889</v>
+      </c>
+      <c r="F27" s="55">
+        <f>DATE(2022, 11, 27)</f>
+        <v>44892</v>
+      </c>
       <c r="G27" s="17"/>
-      <c r="H27" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H27" s="17"/>
       <c r="I27" s="44"/>
       <c r="J27" s="44"/>
       <c r="K27" s="44"/>
@@ -3549,20 +3649,27 @@
       <c r="BK27" s="44"/>
       <c r="BL27" s="44"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="48"/>
-      <c r="B28" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="65"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
+      <c r="B28" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="22">
+        <v>1</v>
+      </c>
+      <c r="E28" s="55">
+        <f>DATE(2022, 11, 21)</f>
+        <v>44886</v>
+      </c>
+      <c r="F28" s="55">
+        <f>DATE(2022, 11, 24)</f>
+        <v>44889</v>
+      </c>
       <c r="G28" s="17"/>
-      <c r="H28" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H28" s="17"/>
       <c r="I28" s="44"/>
       <c r="J28" s="44"/>
       <c r="K28" s="44"/>
@@ -3620,20 +3727,27 @@
       <c r="BK28" s="44"/>
       <c r="BL28" s="44"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="48"/>
-      <c r="B29" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="65"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
+      <c r="B29" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="E29" s="55">
+        <f>DATE(2022, 11, 21)</f>
+        <v>44886</v>
+      </c>
+      <c r="F29" s="55">
+        <f>DATE(2022, 11, 24)</f>
+        <v>44889</v>
+      </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H29" s="17"/>
       <c r="I29" s="44"/>
       <c r="J29" s="44"/>
       <c r="K29" s="44"/>
@@ -3691,15 +3805,17 @@
       <c r="BK29" s="44"/>
       <c r="BL29" s="44"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
-      <c r="B30" s="71" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="62"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="26"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17" t="str">
         <f t="shared" si="6"/>
@@ -3762,17 +3878,15 @@
       <c r="BK30" s="44"/>
       <c r="BL30" s="44"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="66"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="49"/>
+      <c r="B31" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="63"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="17"/>
       <c r="H31" s="17" t="str">
         <f t="shared" si="6"/>
@@ -3835,15 +3949,15 @@
       <c r="BK31" s="44"/>
       <c r="BL31" s="44"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="48"/>
-      <c r="B32" s="72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="67"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
+      <c r="B32" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="63"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17" t="str">
         <f t="shared" si="6"/>
@@ -3861,8 +3975,8 @@
       <c r="R32" s="44"/>
       <c r="S32" s="44"/>
       <c r="T32" s="44"/>
-      <c r="U32" s="44"/>
-      <c r="V32" s="44"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
       <c r="W32" s="44"/>
       <c r="X32" s="44"/>
       <c r="Y32" s="44"/>
@@ -3906,15 +4020,15 @@
       <c r="BK32" s="44"/>
       <c r="BL32" s="44"/>
     </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="48"/>
-      <c r="B33" s="72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
+      <c r="B33" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="63"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
       <c r="G33" s="17"/>
       <c r="H33" s="17" t="str">
         <f t="shared" si="6"/>
@@ -3977,15 +4091,15 @@
       <c r="BK33" s="44"/>
       <c r="BL33" s="44"/>
     </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="48"/>
-      <c r="B34" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="67"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
+      <c r="B34" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="63"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="17"/>
       <c r="H34" s="17" t="str">
         <f t="shared" si="6"/>
@@ -4007,7 +4121,7 @@
       <c r="V34" s="44"/>
       <c r="W34" s="44"/>
       <c r="X34" s="44"/>
-      <c r="Y34" s="44"/>
+      <c r="Y34" s="45"/>
       <c r="Z34" s="44"/>
       <c r="AA34" s="44"/>
       <c r="AB34" s="44"/>
@@ -4048,15 +4162,15 @@
       <c r="BK34" s="44"/>
       <c r="BL34" s="44"/>
     </row>
-    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="48"/>
-      <c r="B35" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="67"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
+      <c r="B35" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="63"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="17"/>
       <c r="H35" s="17" t="str">
         <f t="shared" si="6"/>
@@ -4119,15 +4233,17 @@
       <c r="BK35" s="44"/>
       <c r="BL35" s="44"/>
     </row>
-    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="48"/>
-      <c r="B36" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="67"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
+    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="64"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17" t="str">
         <f t="shared" si="6"/>
@@ -4190,15 +4306,15 @@
       <c r="BK36" s="44"/>
       <c r="BL36" s="44"/>
     </row>
-    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="73"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="48"/>
+      <c r="B37" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="65"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
       <c r="G37" s="17"/>
       <c r="H37" s="17" t="str">
         <f t="shared" si="6"/>
@@ -4261,104 +4377,887 @@
       <c r="BK37" s="44"/>
       <c r="BL37" s="44"/>
     </row>
-    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43" t="str">
+    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="48"/>
+      <c r="B38" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="65"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="46"/>
-      <c r="N38" s="46"/>
-      <c r="O38" s="46"/>
-      <c r="P38" s="46"/>
-      <c r="Q38" s="46"/>
-      <c r="R38" s="46"/>
-      <c r="S38" s="46"/>
-      <c r="T38" s="46"/>
-      <c r="U38" s="46"/>
-      <c r="V38" s="46"/>
-      <c r="W38" s="46"/>
-      <c r="X38" s="46"/>
-      <c r="Y38" s="46"/>
-      <c r="Z38" s="46"/>
-      <c r="AA38" s="46"/>
-      <c r="AB38" s="46"/>
-      <c r="AC38" s="46"/>
-      <c r="AD38" s="46"/>
-      <c r="AE38" s="46"/>
-      <c r="AF38" s="46"/>
-      <c r="AG38" s="46"/>
-      <c r="AH38" s="46"/>
-      <c r="AI38" s="46"/>
-      <c r="AJ38" s="46"/>
-      <c r="AK38" s="46"/>
-      <c r="AL38" s="46"/>
-      <c r="AM38" s="46"/>
-      <c r="AN38" s="46"/>
-      <c r="AO38" s="46"/>
-      <c r="AP38" s="46"/>
-      <c r="AQ38" s="46"/>
-      <c r="AR38" s="46"/>
-      <c r="AS38" s="46"/>
-      <c r="AT38" s="46"/>
-      <c r="AU38" s="46"/>
-      <c r="AV38" s="46"/>
-      <c r="AW38" s="46"/>
-      <c r="AX38" s="46"/>
-      <c r="AY38" s="46"/>
-      <c r="AZ38" s="46"/>
-      <c r="BA38" s="46"/>
-      <c r="BB38" s="46"/>
-      <c r="BC38" s="46"/>
-      <c r="BD38" s="46"/>
-      <c r="BE38" s="46"/>
-      <c r="BF38" s="46"/>
-      <c r="BG38" s="46"/>
-      <c r="BH38" s="46"/>
-      <c r="BI38" s="46"/>
-      <c r="BJ38" s="46"/>
-      <c r="BK38" s="46"/>
-      <c r="BL38" s="46"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="44"/>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
+      <c r="T38" s="44"/>
+      <c r="U38" s="44"/>
+      <c r="V38" s="44"/>
+      <c r="W38" s="44"/>
+      <c r="X38" s="44"/>
+      <c r="Y38" s="44"/>
+      <c r="Z38" s="44"/>
+      <c r="AA38" s="44"/>
+      <c r="AB38" s="44"/>
+      <c r="AC38" s="44"/>
+      <c r="AD38" s="44"/>
+      <c r="AE38" s="44"/>
+      <c r="AF38" s="44"/>
+      <c r="AG38" s="44"/>
+      <c r="AH38" s="44"/>
+      <c r="AI38" s="44"/>
+      <c r="AJ38" s="44"/>
+      <c r="AK38" s="44"/>
+      <c r="AL38" s="44"/>
+      <c r="AM38" s="44"/>
+      <c r="AN38" s="44"/>
+      <c r="AO38" s="44"/>
+      <c r="AP38" s="44"/>
+      <c r="AQ38" s="44"/>
+      <c r="AR38" s="44"/>
+      <c r="AS38" s="44"/>
+      <c r="AT38" s="44"/>
+      <c r="AU38" s="44"/>
+      <c r="AV38" s="44"/>
+      <c r="AW38" s="44"/>
+      <c r="AX38" s="44"/>
+      <c r="AY38" s="44"/>
+      <c r="AZ38" s="44"/>
+      <c r="BA38" s="44"/>
+      <c r="BB38" s="44"/>
+      <c r="BC38" s="44"/>
+      <c r="BD38" s="44"/>
+      <c r="BE38" s="44"/>
+      <c r="BF38" s="44"/>
+      <c r="BG38" s="44"/>
+      <c r="BH38" s="44"/>
+      <c r="BI38" s="44"/>
+      <c r="BJ38" s="44"/>
+      <c r="BK38" s="44"/>
+      <c r="BL38" s="44"/>
     </row>
-    <row r="39" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G39" s="6"/>
+    <row r="39" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="48"/>
+      <c r="B39" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="65"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="44"/>
+      <c r="X39" s="44"/>
+      <c r="Y39" s="44"/>
+      <c r="Z39" s="44"/>
+      <c r="AA39" s="44"/>
+      <c r="AB39" s="44"/>
+      <c r="AC39" s="44"/>
+      <c r="AD39" s="44"/>
+      <c r="AE39" s="44"/>
+      <c r="AF39" s="44"/>
+      <c r="AG39" s="44"/>
+      <c r="AH39" s="44"/>
+      <c r="AI39" s="44"/>
+      <c r="AJ39" s="44"/>
+      <c r="AK39" s="44"/>
+      <c r="AL39" s="44"/>
+      <c r="AM39" s="44"/>
+      <c r="AN39" s="44"/>
+      <c r="AO39" s="44"/>
+      <c r="AP39" s="44"/>
+      <c r="AQ39" s="44"/>
+      <c r="AR39" s="44"/>
+      <c r="AS39" s="44"/>
+      <c r="AT39" s="44"/>
+      <c r="AU39" s="44"/>
+      <c r="AV39" s="44"/>
+      <c r="AW39" s="44"/>
+      <c r="AX39" s="44"/>
+      <c r="AY39" s="44"/>
+      <c r="AZ39" s="44"/>
+      <c r="BA39" s="44"/>
+      <c r="BB39" s="44"/>
+      <c r="BC39" s="44"/>
+      <c r="BD39" s="44"/>
+      <c r="BE39" s="44"/>
+      <c r="BF39" s="44"/>
+      <c r="BG39" s="44"/>
+      <c r="BH39" s="44"/>
+      <c r="BI39" s="44"/>
+      <c r="BJ39" s="44"/>
+      <c r="BK39" s="44"/>
+      <c r="BL39" s="44"/>
     </row>
-    <row r="40" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="14"/>
-      <c r="F40" s="50"/>
+    <row r="40" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="48"/>
+      <c r="B40" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="65"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="44"/>
+      <c r="N40" s="44"/>
+      <c r="O40" s="44"/>
+      <c r="P40" s="44"/>
+      <c r="Q40" s="44"/>
+      <c r="R40" s="44"/>
+      <c r="S40" s="44"/>
+      <c r="T40" s="44"/>
+      <c r="U40" s="44"/>
+      <c r="V40" s="44"/>
+      <c r="W40" s="44"/>
+      <c r="X40" s="44"/>
+      <c r="Y40" s="44"/>
+      <c r="Z40" s="44"/>
+      <c r="AA40" s="44"/>
+      <c r="AB40" s="44"/>
+      <c r="AC40" s="44"/>
+      <c r="AD40" s="44"/>
+      <c r="AE40" s="44"/>
+      <c r="AF40" s="44"/>
+      <c r="AG40" s="44"/>
+      <c r="AH40" s="44"/>
+      <c r="AI40" s="44"/>
+      <c r="AJ40" s="44"/>
+      <c r="AK40" s="44"/>
+      <c r="AL40" s="44"/>
+      <c r="AM40" s="44"/>
+      <c r="AN40" s="44"/>
+      <c r="AO40" s="44"/>
+      <c r="AP40" s="44"/>
+      <c r="AQ40" s="44"/>
+      <c r="AR40" s="44"/>
+      <c r="AS40" s="44"/>
+      <c r="AT40" s="44"/>
+      <c r="AU40" s="44"/>
+      <c r="AV40" s="44"/>
+      <c r="AW40" s="44"/>
+      <c r="AX40" s="44"/>
+      <c r="AY40" s="44"/>
+      <c r="AZ40" s="44"/>
+      <c r="BA40" s="44"/>
+      <c r="BB40" s="44"/>
+      <c r="BC40" s="44"/>
+      <c r="BD40" s="44"/>
+      <c r="BE40" s="44"/>
+      <c r="BF40" s="44"/>
+      <c r="BG40" s="44"/>
+      <c r="BH40" s="44"/>
+      <c r="BI40" s="44"/>
+      <c r="BJ40" s="44"/>
+      <c r="BK40" s="44"/>
+      <c r="BL40" s="44"/>
     </row>
-    <row r="41" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="15"/>
+    <row r="41" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="48"/>
+      <c r="B41" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="65"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="44"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="44"/>
+      <c r="W41" s="44"/>
+      <c r="X41" s="44"/>
+      <c r="Y41" s="44"/>
+      <c r="Z41" s="44"/>
+      <c r="AA41" s="44"/>
+      <c r="AB41" s="44"/>
+      <c r="AC41" s="44"/>
+      <c r="AD41" s="44"/>
+      <c r="AE41" s="44"/>
+      <c r="AF41" s="44"/>
+      <c r="AG41" s="44"/>
+      <c r="AH41" s="44"/>
+      <c r="AI41" s="44"/>
+      <c r="AJ41" s="44"/>
+      <c r="AK41" s="44"/>
+      <c r="AL41" s="44"/>
+      <c r="AM41" s="44"/>
+      <c r="AN41" s="44"/>
+      <c r="AO41" s="44"/>
+      <c r="AP41" s="44"/>
+      <c r="AQ41" s="44"/>
+      <c r="AR41" s="44"/>
+      <c r="AS41" s="44"/>
+      <c r="AT41" s="44"/>
+      <c r="AU41" s="44"/>
+      <c r="AV41" s="44"/>
+      <c r="AW41" s="44"/>
+      <c r="AX41" s="44"/>
+      <c r="AY41" s="44"/>
+      <c r="AZ41" s="44"/>
+      <c r="BA41" s="44"/>
+      <c r="BB41" s="44"/>
+      <c r="BC41" s="44"/>
+      <c r="BD41" s="44"/>
+      <c r="BE41" s="44"/>
+      <c r="BF41" s="44"/>
+      <c r="BG41" s="44"/>
+      <c r="BH41" s="44"/>
+      <c r="BI41" s="44"/>
+      <c r="BJ41" s="44"/>
+      <c r="BK41" s="44"/>
+      <c r="BL41" s="44"/>
+    </row>
+    <row r="42" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="66"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="44"/>
+      <c r="S42" s="44"/>
+      <c r="T42" s="44"/>
+      <c r="U42" s="44"/>
+      <c r="V42" s="44"/>
+      <c r="W42" s="44"/>
+      <c r="X42" s="44"/>
+      <c r="Y42" s="44"/>
+      <c r="Z42" s="44"/>
+      <c r="AA42" s="44"/>
+      <c r="AB42" s="44"/>
+      <c r="AC42" s="44"/>
+      <c r="AD42" s="44"/>
+      <c r="AE42" s="44"/>
+      <c r="AF42" s="44"/>
+      <c r="AG42" s="44"/>
+      <c r="AH42" s="44"/>
+      <c r="AI42" s="44"/>
+      <c r="AJ42" s="44"/>
+      <c r="AK42" s="44"/>
+      <c r="AL42" s="44"/>
+      <c r="AM42" s="44"/>
+      <c r="AN42" s="44"/>
+      <c r="AO42" s="44"/>
+      <c r="AP42" s="44"/>
+      <c r="AQ42" s="44"/>
+      <c r="AR42" s="44"/>
+      <c r="AS42" s="44"/>
+      <c r="AT42" s="44"/>
+      <c r="AU42" s="44"/>
+      <c r="AV42" s="44"/>
+      <c r="AW42" s="44"/>
+      <c r="AX42" s="44"/>
+      <c r="AY42" s="44"/>
+      <c r="AZ42" s="44"/>
+      <c r="BA42" s="44"/>
+      <c r="BB42" s="44"/>
+      <c r="BC42" s="44"/>
+      <c r="BD42" s="44"/>
+      <c r="BE42" s="44"/>
+      <c r="BF42" s="44"/>
+      <c r="BG42" s="44"/>
+      <c r="BH42" s="44"/>
+      <c r="BI42" s="44"/>
+      <c r="BJ42" s="44"/>
+      <c r="BK42" s="44"/>
+      <c r="BL42" s="44"/>
+    </row>
+    <row r="43" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="48"/>
+      <c r="B43" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="67"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="44"/>
+      <c r="V43" s="44"/>
+      <c r="W43" s="44"/>
+      <c r="X43" s="44"/>
+      <c r="Y43" s="44"/>
+      <c r="Z43" s="44"/>
+      <c r="AA43" s="44"/>
+      <c r="AB43" s="44"/>
+      <c r="AC43" s="44"/>
+      <c r="AD43" s="44"/>
+      <c r="AE43" s="44"/>
+      <c r="AF43" s="44"/>
+      <c r="AG43" s="44"/>
+      <c r="AH43" s="44"/>
+      <c r="AI43" s="44"/>
+      <c r="AJ43" s="44"/>
+      <c r="AK43" s="44"/>
+      <c r="AL43" s="44"/>
+      <c r="AM43" s="44"/>
+      <c r="AN43" s="44"/>
+      <c r="AO43" s="44"/>
+      <c r="AP43" s="44"/>
+      <c r="AQ43" s="44"/>
+      <c r="AR43" s="44"/>
+      <c r="AS43" s="44"/>
+      <c r="AT43" s="44"/>
+      <c r="AU43" s="44"/>
+      <c r="AV43" s="44"/>
+      <c r="AW43" s="44"/>
+      <c r="AX43" s="44"/>
+      <c r="AY43" s="44"/>
+      <c r="AZ43" s="44"/>
+      <c r="BA43" s="44"/>
+      <c r="BB43" s="44"/>
+      <c r="BC43" s="44"/>
+      <c r="BD43" s="44"/>
+      <c r="BE43" s="44"/>
+      <c r="BF43" s="44"/>
+      <c r="BG43" s="44"/>
+      <c r="BH43" s="44"/>
+      <c r="BI43" s="44"/>
+      <c r="BJ43" s="44"/>
+      <c r="BK43" s="44"/>
+      <c r="BL43" s="44"/>
+    </row>
+    <row r="44" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="48"/>
+      <c r="B44" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="67"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44"/>
+      <c r="O44" s="44"/>
+      <c r="P44" s="44"/>
+      <c r="Q44" s="44"/>
+      <c r="R44" s="44"/>
+      <c r="S44" s="44"/>
+      <c r="T44" s="44"/>
+      <c r="U44" s="44"/>
+      <c r="V44" s="44"/>
+      <c r="W44" s="44"/>
+      <c r="X44" s="44"/>
+      <c r="Y44" s="44"/>
+      <c r="Z44" s="44"/>
+      <c r="AA44" s="44"/>
+      <c r="AB44" s="44"/>
+      <c r="AC44" s="44"/>
+      <c r="AD44" s="44"/>
+      <c r="AE44" s="44"/>
+      <c r="AF44" s="44"/>
+      <c r="AG44" s="44"/>
+      <c r="AH44" s="44"/>
+      <c r="AI44" s="44"/>
+      <c r="AJ44" s="44"/>
+      <c r="AK44" s="44"/>
+      <c r="AL44" s="44"/>
+      <c r="AM44" s="44"/>
+      <c r="AN44" s="44"/>
+      <c r="AO44" s="44"/>
+      <c r="AP44" s="44"/>
+      <c r="AQ44" s="44"/>
+      <c r="AR44" s="44"/>
+      <c r="AS44" s="44"/>
+      <c r="AT44" s="44"/>
+      <c r="AU44" s="44"/>
+      <c r="AV44" s="44"/>
+      <c r="AW44" s="44"/>
+      <c r="AX44" s="44"/>
+      <c r="AY44" s="44"/>
+      <c r="AZ44" s="44"/>
+      <c r="BA44" s="44"/>
+      <c r="BB44" s="44"/>
+      <c r="BC44" s="44"/>
+      <c r="BD44" s="44"/>
+      <c r="BE44" s="44"/>
+      <c r="BF44" s="44"/>
+      <c r="BG44" s="44"/>
+      <c r="BH44" s="44"/>
+      <c r="BI44" s="44"/>
+      <c r="BJ44" s="44"/>
+      <c r="BK44" s="44"/>
+      <c r="BL44" s="44"/>
+    </row>
+    <row r="45" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="48"/>
+      <c r="B45" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="67"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="44"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="44"/>
+      <c r="P45" s="44"/>
+      <c r="Q45" s="44"/>
+      <c r="R45" s="44"/>
+      <c r="S45" s="44"/>
+      <c r="T45" s="44"/>
+      <c r="U45" s="44"/>
+      <c r="V45" s="44"/>
+      <c r="W45" s="44"/>
+      <c r="X45" s="44"/>
+      <c r="Y45" s="44"/>
+      <c r="Z45" s="44"/>
+      <c r="AA45" s="44"/>
+      <c r="AB45" s="44"/>
+      <c r="AC45" s="44"/>
+      <c r="AD45" s="44"/>
+      <c r="AE45" s="44"/>
+      <c r="AF45" s="44"/>
+      <c r="AG45" s="44"/>
+      <c r="AH45" s="44"/>
+      <c r="AI45" s="44"/>
+      <c r="AJ45" s="44"/>
+      <c r="AK45" s="44"/>
+      <c r="AL45" s="44"/>
+      <c r="AM45" s="44"/>
+      <c r="AN45" s="44"/>
+      <c r="AO45" s="44"/>
+      <c r="AP45" s="44"/>
+      <c r="AQ45" s="44"/>
+      <c r="AR45" s="44"/>
+      <c r="AS45" s="44"/>
+      <c r="AT45" s="44"/>
+      <c r="AU45" s="44"/>
+      <c r="AV45" s="44"/>
+      <c r="AW45" s="44"/>
+      <c r="AX45" s="44"/>
+      <c r="AY45" s="44"/>
+      <c r="AZ45" s="44"/>
+      <c r="BA45" s="44"/>
+      <c r="BB45" s="44"/>
+      <c r="BC45" s="44"/>
+      <c r="BD45" s="44"/>
+      <c r="BE45" s="44"/>
+      <c r="BF45" s="44"/>
+      <c r="BG45" s="44"/>
+      <c r="BH45" s="44"/>
+      <c r="BI45" s="44"/>
+      <c r="BJ45" s="44"/>
+      <c r="BK45" s="44"/>
+      <c r="BL45" s="44"/>
+    </row>
+    <row r="46" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="48"/>
+      <c r="B46" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="67"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="44"/>
+      <c r="O46" s="44"/>
+      <c r="P46" s="44"/>
+      <c r="Q46" s="44"/>
+      <c r="R46" s="44"/>
+      <c r="S46" s="44"/>
+      <c r="T46" s="44"/>
+      <c r="U46" s="44"/>
+      <c r="V46" s="44"/>
+      <c r="W46" s="44"/>
+      <c r="X46" s="44"/>
+      <c r="Y46" s="44"/>
+      <c r="Z46" s="44"/>
+      <c r="AA46" s="44"/>
+      <c r="AB46" s="44"/>
+      <c r="AC46" s="44"/>
+      <c r="AD46" s="44"/>
+      <c r="AE46" s="44"/>
+      <c r="AF46" s="44"/>
+      <c r="AG46" s="44"/>
+      <c r="AH46" s="44"/>
+      <c r="AI46" s="44"/>
+      <c r="AJ46" s="44"/>
+      <c r="AK46" s="44"/>
+      <c r="AL46" s="44"/>
+      <c r="AM46" s="44"/>
+      <c r="AN46" s="44"/>
+      <c r="AO46" s="44"/>
+      <c r="AP46" s="44"/>
+      <c r="AQ46" s="44"/>
+      <c r="AR46" s="44"/>
+      <c r="AS46" s="44"/>
+      <c r="AT46" s="44"/>
+      <c r="AU46" s="44"/>
+      <c r="AV46" s="44"/>
+      <c r="AW46" s="44"/>
+      <c r="AX46" s="44"/>
+      <c r="AY46" s="44"/>
+      <c r="AZ46" s="44"/>
+      <c r="BA46" s="44"/>
+      <c r="BB46" s="44"/>
+      <c r="BC46" s="44"/>
+      <c r="BD46" s="44"/>
+      <c r="BE46" s="44"/>
+      <c r="BF46" s="44"/>
+      <c r="BG46" s="44"/>
+      <c r="BH46" s="44"/>
+      <c r="BI46" s="44"/>
+      <c r="BJ46" s="44"/>
+      <c r="BK46" s="44"/>
+      <c r="BL46" s="44"/>
+    </row>
+    <row r="47" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="48"/>
+      <c r="B47" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="67"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="44"/>
+      <c r="O47" s="44"/>
+      <c r="P47" s="44"/>
+      <c r="Q47" s="44"/>
+      <c r="R47" s="44"/>
+      <c r="S47" s="44"/>
+      <c r="T47" s="44"/>
+      <c r="U47" s="44"/>
+      <c r="V47" s="44"/>
+      <c r="W47" s="44"/>
+      <c r="X47" s="44"/>
+      <c r="Y47" s="44"/>
+      <c r="Z47" s="44"/>
+      <c r="AA47" s="44"/>
+      <c r="AB47" s="44"/>
+      <c r="AC47" s="44"/>
+      <c r="AD47" s="44"/>
+      <c r="AE47" s="44"/>
+      <c r="AF47" s="44"/>
+      <c r="AG47" s="44"/>
+      <c r="AH47" s="44"/>
+      <c r="AI47" s="44"/>
+      <c r="AJ47" s="44"/>
+      <c r="AK47" s="44"/>
+      <c r="AL47" s="44"/>
+      <c r="AM47" s="44"/>
+      <c r="AN47" s="44"/>
+      <c r="AO47" s="44"/>
+      <c r="AP47" s="44"/>
+      <c r="AQ47" s="44"/>
+      <c r="AR47" s="44"/>
+      <c r="AS47" s="44"/>
+      <c r="AT47" s="44"/>
+      <c r="AU47" s="44"/>
+      <c r="AV47" s="44"/>
+      <c r="AW47" s="44"/>
+      <c r="AX47" s="44"/>
+      <c r="AY47" s="44"/>
+      <c r="AZ47" s="44"/>
+      <c r="BA47" s="44"/>
+      <c r="BB47" s="44"/>
+      <c r="BC47" s="44"/>
+      <c r="BD47" s="44"/>
+      <c r="BE47" s="44"/>
+      <c r="BF47" s="44"/>
+      <c r="BG47" s="44"/>
+      <c r="BH47" s="44"/>
+      <c r="BI47" s="44"/>
+      <c r="BJ47" s="44"/>
+      <c r="BK47" s="44"/>
+      <c r="BL47" s="44"/>
+    </row>
+    <row r="48" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="73"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
+      <c r="M48" s="44"/>
+      <c r="N48" s="44"/>
+      <c r="O48" s="44"/>
+      <c r="P48" s="44"/>
+      <c r="Q48" s="44"/>
+      <c r="R48" s="44"/>
+      <c r="S48" s="44"/>
+      <c r="T48" s="44"/>
+      <c r="U48" s="44"/>
+      <c r="V48" s="44"/>
+      <c r="W48" s="44"/>
+      <c r="X48" s="44"/>
+      <c r="Y48" s="44"/>
+      <c r="Z48" s="44"/>
+      <c r="AA48" s="44"/>
+      <c r="AB48" s="44"/>
+      <c r="AC48" s="44"/>
+      <c r="AD48" s="44"/>
+      <c r="AE48" s="44"/>
+      <c r="AF48" s="44"/>
+      <c r="AG48" s="44"/>
+      <c r="AH48" s="44"/>
+      <c r="AI48" s="44"/>
+      <c r="AJ48" s="44"/>
+      <c r="AK48" s="44"/>
+      <c r="AL48" s="44"/>
+      <c r="AM48" s="44"/>
+      <c r="AN48" s="44"/>
+      <c r="AO48" s="44"/>
+      <c r="AP48" s="44"/>
+      <c r="AQ48" s="44"/>
+      <c r="AR48" s="44"/>
+      <c r="AS48" s="44"/>
+      <c r="AT48" s="44"/>
+      <c r="AU48" s="44"/>
+      <c r="AV48" s="44"/>
+      <c r="AW48" s="44"/>
+      <c r="AX48" s="44"/>
+      <c r="AY48" s="44"/>
+      <c r="AZ48" s="44"/>
+      <c r="BA48" s="44"/>
+      <c r="BB48" s="44"/>
+      <c r="BC48" s="44"/>
+      <c r="BD48" s="44"/>
+      <c r="BE48" s="44"/>
+      <c r="BF48" s="44"/>
+      <c r="BG48" s="44"/>
+      <c r="BH48" s="44"/>
+      <c r="BI48" s="44"/>
+      <c r="BJ48" s="44"/>
+      <c r="BK48" s="44"/>
+      <c r="BL48" s="44"/>
+    </row>
+    <row r="49" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="39"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+      <c r="M49" s="46"/>
+      <c r="N49" s="46"/>
+      <c r="O49" s="46"/>
+      <c r="P49" s="46"/>
+      <c r="Q49" s="46"/>
+      <c r="R49" s="46"/>
+      <c r="S49" s="46"/>
+      <c r="T49" s="46"/>
+      <c r="U49" s="46"/>
+      <c r="V49" s="46"/>
+      <c r="W49" s="46"/>
+      <c r="X49" s="46"/>
+      <c r="Y49" s="46"/>
+      <c r="Z49" s="46"/>
+      <c r="AA49" s="46"/>
+      <c r="AB49" s="46"/>
+      <c r="AC49" s="46"/>
+      <c r="AD49" s="46"/>
+      <c r="AE49" s="46"/>
+      <c r="AF49" s="46"/>
+      <c r="AG49" s="46"/>
+      <c r="AH49" s="46"/>
+      <c r="AI49" s="46"/>
+      <c r="AJ49" s="46"/>
+      <c r="AK49" s="46"/>
+      <c r="AL49" s="46"/>
+      <c r="AM49" s="46"/>
+      <c r="AN49" s="46"/>
+      <c r="AO49" s="46"/>
+      <c r="AP49" s="46"/>
+      <c r="AQ49" s="46"/>
+      <c r="AR49" s="46"/>
+      <c r="AS49" s="46"/>
+      <c r="AT49" s="46"/>
+      <c r="AU49" s="46"/>
+      <c r="AV49" s="46"/>
+      <c r="AW49" s="46"/>
+      <c r="AX49" s="46"/>
+      <c r="AY49" s="46"/>
+      <c r="AZ49" s="46"/>
+      <c r="BA49" s="46"/>
+      <c r="BB49" s="46"/>
+      <c r="BC49" s="46"/>
+      <c r="BD49" s="46"/>
+      <c r="BE49" s="46"/>
+      <c r="BF49" s="46"/>
+      <c r="BG49" s="46"/>
+      <c r="BH49" s="46"/>
+      <c r="BI49" s="46"/>
+      <c r="BJ49" s="46"/>
+      <c r="BK49" s="46"/>
+      <c r="BL49" s="46"/>
+    </row>
+    <row r="50" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C51" s="14"/>
+      <c r="F51" s="50"/>
+    </row>
+    <row r="52" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C52" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D38">
+  <conditionalFormatting sqref="D7:D49">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4372,12 +5271,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL38">
+  <conditionalFormatting sqref="I5:BL49">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL38">
+  <conditionalFormatting sqref="I7:BL49">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4412,7 +5311,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D38</xm:sqref>
+          <xm:sqref>D7:D49</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>